<commit_message>
Adds missing fuels for REMIND scenarios (coal-based). Adds inventories for bioethanol and biodiesel from Cavalett & Cherubini, 2022. Updated coal-based hydrogen and adds CCS option.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-coal-gasification.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-coal-gasification.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0623BE0-A57D-5A4D-80C0-08D42927AFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6710E4D6-8A17-BE4B-9A51-9F74F63414F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$25</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateCount="10" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="84">
   <si>
     <t>Activity</t>
   </si>
@@ -91,9 +91,6 @@
     <t>biosphere</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Carbon dioxide, fossil</t>
   </si>
   <si>
@@ -160,15 +157,9 @@
     <t>market group for electricity, medium voltage</t>
   </si>
   <si>
-    <t>ENTSO-E</t>
-  </si>
-  <si>
     <t>kilowatt hour</t>
   </si>
   <si>
-    <t>updated UCTE medium voltage supply with ENTSO-E high voltage supply due to updates in ecoinvent</t>
-  </si>
-  <si>
     <t>electricity, medium voltage</t>
   </si>
   <si>
@@ -199,18 +190,12 @@
     <t>water, deionised</t>
   </si>
   <si>
-    <t>Originally in megajoule. LHV: 120 MJ/kg.</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
     <t>Europe, without Russia and Turkey</t>
   </si>
   <si>
-    <t>Wokaun A, Wilhelm E, Schenler W, Simons A, Bauer C, Bond S, et al. Transition to hydrogen - pathways toward clean transportation. New York: Cambridge University Press; 2011</t>
-  </si>
-  <si>
     <t>Hydrogen from coal Gasification</t>
   </si>
   <si>
@@ -218,6 +203,91 @@
   </si>
   <si>
     <t>hydrogen production, gaseous, 30 bar, from hard coal gasification and reforming, at coal gasification plant</t>
+  </si>
+  <si>
+    <t>Originally: Wokaun A, Wilhelm E, Schenler W, Simons A, Bauer C, Bond S, et al. Transition to hydrogen - pathways toward clean transportation. New York: Cambridge University Press; 2011
+Updated with: Jiaquan Li, Yi-Ming Wei, Lancui Liu, Xiaoyu Li, Rui Yan, The carbon footprint and cost of coal-based hydrogen production with and without carbon capture and storage technology in China, Journal of Cleaner Production, 2022, https://doi.org/10.1016/j.jclepro.2022.132514.</t>
+  </si>
+  <si>
+    <t>Originally in megajoule. LHV: 120 MJ/kg. Originally: Wokaun A, Wilhelm E, Schenler W, Simons A, Bauer C, Bond S, et al. Transition to hydrogen - pathways toward clean transportation. New York: Cambridge University Press; 2011. Updated with: Jiaquan Li, Yi-Ming Wei, Lancui Liu, Xiaoyu Li, Rui Yan, The carbon footprint and cost of coal-based hydrogen production with and without carbon capture and storage technology in China, Journal of Cleaner Production, 2022, https://doi.org/10.1016/j.jclepro.2022.132514.</t>
+  </si>
+  <si>
+    <t>From Wokaun et al., 2011.</t>
+  </si>
+  <si>
+    <t>From Li et al., 2022.</t>
+  </si>
+  <si>
+    <t>market for aluminium oxide, metallurgical</t>
+  </si>
+  <si>
+    <t>IAI Area, EU27 &amp; EFTA</t>
+  </si>
+  <si>
+    <t>aluminium oxide, metallurgical</t>
+  </si>
+  <si>
+    <t>methanol distillation, hydrogen from coal gasification</t>
+  </si>
+  <si>
+    <t>methanol, purified</t>
+  </si>
+  <si>
+    <t>treatment of wastewater, average, capacity 1E9l/year</t>
+  </si>
+  <si>
+    <t>cubic meter</t>
+  </si>
+  <si>
+    <t>wastewater, average</t>
+  </si>
+  <si>
+    <t>From Li et al., 2022. For CCS.</t>
+  </si>
+  <si>
+    <t>market for tap water</t>
+  </si>
+  <si>
+    <t>RoW</t>
+  </si>
+  <si>
+    <t>tap water</t>
+  </si>
+  <si>
+    <t>From Li et al., 2022. For CCS. Originally called "cooling water", hence, may be from river or even the sea.</t>
+  </si>
+  <si>
+    <t>market for ammonia, anhydrous, liquid</t>
+  </si>
+  <si>
+    <t>ammonia, anhydrous, liquid</t>
+  </si>
+  <si>
+    <t>nitrogen, liquid</t>
+  </si>
+  <si>
+    <t>market for nitrogen, liquid</t>
+  </si>
+  <si>
+    <t>Volkart et al., 2013</t>
+  </si>
+  <si>
+    <t>Originally in megajoule. LHV: 120 MJ/kg. Originally: Wokaun A, Wilhelm E, Schenler W, Simons A, Bauer C, Bond S, et al. Transition to hydrogen - pathways toward clean transportation. New York: Cambridge University Press; 2011. Updated with: Jiaquan Li, Yi-Ming Wei, Lancui Liu, Xiaoyu Li, Rui Yan, The carbon footprint and cost of coal-based hydrogen production with and without carbon capture and storage technology in China, Journal of Cleaner Production, 2022, https://doi.org/10.1016/j.jclepro.2022.132514. Li et al., 2022, is based on an existing plant in China, and an existing CCS project in China. CO2 transport and storage is from Volkart et al., 2013.</t>
+  </si>
+  <si>
+    <t>Water, cooling, unspecified natural origin</t>
+  </si>
+  <si>
+    <t>natural resource::in water</t>
+  </si>
+  <si>
+    <t>From Li et al., 2022. For CCS. Originally called "desalted water", hence, desalination process is missing.</t>
+  </si>
+  <si>
+    <t>CO2 storage/hard coal, post, pipeline 200km, storage 1000m</t>
+  </si>
+  <si>
+    <t>hydrogen production, gaseous, 30 bar, from hard coal gasification and reforming, with CCS, at coal gasification plant</t>
   </si>
 </sst>
 </file>
@@ -275,11 +345,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,25 +632,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="54.5" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -586,7 +660,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -602,7 +676,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -626,7 +700,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -634,15 +708,15 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" t="s">
-        <v>57</v>
+        <v>51</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -682,293 +756,295 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>14</v>
+    <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="B13">
-        <v>6.9264000000000001E-3</v>
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
       </c>
-      <c r="E13" t="s">
-        <v>16</v>
-      </c>
       <c r="F13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>5.7720000000000003E-5</v>
+        <v>20</v>
       </c>
       <c r="I13" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="B14">
-        <v>18.024000000000001</v>
+        <v>10.5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
       </c>
-      <c r="E14" t="s">
-        <v>16</v>
-      </c>
       <c r="F14" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <v>0.1502</v>
+        <v>7.7829999999999996E-2</v>
       </c>
       <c r="I14" t="s">
-        <v>18</v>
+        <v>59</v>
+      </c>
+      <c r="J14" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B15">
-        <v>1.0375199999999999E-2</v>
+        <v>6.9971999999999994E-10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>8.6459999999999996E-5</v>
+        <v>5.8309999999999997E-12</v>
       </c>
       <c r="I15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>60</v>
+        <v>25</v>
+      </c>
+      <c r="J15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>27</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0.16752</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>1.3960000000000001E-3</v>
       </c>
       <c r="I16" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="J16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B17">
-        <v>6.9971999999999994E-10</v>
+        <v>3.9743999999999998E-9</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
       </c>
       <c r="F17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>5.8309999999999997E-12</v>
+        <v>3.3119999999999998E-11</v>
       </c>
       <c r="I17" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="J17" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B18">
-        <v>0.16752</v>
-      </c>
-      <c r="C18" t="s">
-        <v>29</v>
+        <v>8.9</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="D18" t="s">
         <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <v>1.3960000000000001E-3</v>
+        <v>5.6059999999999999E-2</v>
       </c>
       <c r="I18" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="J18" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B19">
-        <v>3.9743999999999998E-9</v>
+        <v>1.1397599999999999</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>3.3119999999999998E-11</v>
+        <v>9.4979999999999995E-3</v>
       </c>
       <c r="I19" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="J19" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B20">
-        <v>6.7271999999999998</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>56</v>
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="F20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>5.6059999999999999E-2</v>
+        <v>2.3179999999999999E-2</v>
+      </c>
+      <c r="I20" t="s">
+        <v>59</v>
       </c>
       <c r="J20" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="B21">
-        <v>1.1397599999999999</v>
+        <f>0.98/1000</f>
+        <v>9.7999999999999997E-4</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="F21" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>9.4979999999999995E-3</v>
+        <v>24</v>
       </c>
       <c r="I21" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="J21" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="B22">
-        <v>2.7816000000000001</v>
+        <f>4.44/1000</f>
+        <v>4.4400000000000004E-3</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="F22" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>2.3179999999999999E-2</v>
+        <v>24</v>
       </c>
       <c r="I22" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="J22" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B23">
         <v>0.42432000000000003</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -977,27 +1053,27 @@
         <v>3.5360000000000001E-3</v>
       </c>
       <c r="I23" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="J23" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B24">
         <v>-0.50531999999999999</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D24" t="s">
         <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -1006,27 +1082,27 @@
         <v>4.2110000000000003E-3</v>
       </c>
       <c r="I24" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="J24" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B25">
         <v>-0.22847999999999999</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" t="s">
         <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -1035,43 +1111,828 @@
         <v>1.9040000000000001E-3</v>
       </c>
       <c r="I25" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="J25" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="5">
+        <f>-36.07/1000</f>
+        <v>-3.6069999999999998E-2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" t="s">
+        <v>59</v>
+      </c>
+      <c r="J26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <v>6.9264000000000001E-3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>5.7720000000000003E-5</v>
+      </c>
+      <c r="I27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28">
+        <v>17.77</v>
+      </c>
+      <c r="D28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0.1502</v>
+      </c>
+      <c r="I28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29">
+        <v>1.0375199999999999E-2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>8.6459999999999996E-5</v>
+      </c>
+      <c r="I29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" t="s">
+        <v>3</v>
+      </c>
+      <c r="G40" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" t="s">
+        <v>12</v>
+      </c>
+      <c r="I40" t="s">
+        <v>13</v>
+      </c>
+      <c r="J40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" t="s">
+        <v>20</v>
+      </c>
+      <c r="I41" t="s">
+        <v>21</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42">
+        <v>10.5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" t="s">
+        <v>24</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>7.7829999999999996E-2</v>
+      </c>
+      <c r="I42" t="s">
+        <v>59</v>
+      </c>
+      <c r="J42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43">
+        <f>32/1000</f>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" t="s">
+        <v>80</v>
+      </c>
+      <c r="F43" t="s">
+        <v>17</v>
+      </c>
+      <c r="I43" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44">
+        <v>10.24</v>
+      </c>
+      <c r="C44" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" t="s">
+        <v>24</v>
+      </c>
+      <c r="I44" t="s">
+        <v>81</v>
+      </c>
+      <c r="J44" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45">
+        <f>0.008*1.2</f>
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" t="s">
+        <v>24</v>
+      </c>
+      <c r="I45" t="s">
+        <v>72</v>
+      </c>
+      <c r="J45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46">
+        <f>0.057/1000</f>
+        <v>5.7000000000000003E-5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" t="s">
+        <v>24</v>
+      </c>
+      <c r="I46" t="s">
+        <v>72</v>
+      </c>
+      <c r="J46" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47">
+        <v>6.9971999999999994E-10</v>
+      </c>
+      <c r="C47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47" t="s">
+        <v>24</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>5.8309999999999997E-12</v>
+      </c>
+      <c r="I47" t="s">
+        <v>25</v>
+      </c>
+      <c r="J47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48">
+        <v>0.16752</v>
+      </c>
+      <c r="C48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" t="s">
+        <v>24</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>1.3960000000000001E-3</v>
+      </c>
+      <c r="I48" t="s">
+        <v>58</v>
+      </c>
+      <c r="J48" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49">
+        <v>3.9743999999999998E-9</v>
+      </c>
+      <c r="C49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D49" t="s">
+        <v>5</v>
+      </c>
+      <c r="F49" t="s">
+        <v>24</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>3.3119999999999998E-11</v>
+      </c>
+      <c r="I49" t="s">
+        <v>31</v>
+      </c>
+      <c r="J49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50">
+        <v>8.9</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B26">
-        <v>9.339599999999999</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="D50" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" t="s">
+        <v>24</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>5.6059999999999999E-2</v>
+      </c>
+      <c r="I50" t="s">
+        <v>59</v>
+      </c>
+      <c r="J50" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>35</v>
+      </c>
+      <c r="B51">
+        <v>1.1397599999999999</v>
+      </c>
+      <c r="C51" t="s">
+        <v>36</v>
+      </c>
+      <c r="D51" t="s">
         <v>37</v>
       </c>
-      <c r="D26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" t="s">
-        <v>25</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>7.7829999999999996E-2</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="F51" t="s">
+        <v>24</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>9.4979999999999995E-3</v>
+      </c>
+      <c r="I51" t="s">
+        <v>58</v>
+      </c>
+      <c r="J51" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>39</v>
+      </c>
+      <c r="B52">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="C52" t="s">
+        <v>36</v>
+      </c>
+      <c r="D52" t="s">
+        <v>40</v>
+      </c>
+      <c r="F52" t="s">
+        <v>24</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>2.3179999999999999E-2</v>
+      </c>
+      <c r="I52" t="s">
+        <v>59</v>
+      </c>
+      <c r="J52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>39</v>
+      </c>
+      <c r="B53">
+        <v>3.36</v>
+      </c>
+      <c r="C53" t="s">
+        <v>36</v>
+      </c>
+      <c r="D53" t="s">
+        <v>40</v>
+      </c>
+      <c r="F53" t="s">
+        <v>24</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>2.3179999999999999E-2</v>
+      </c>
+      <c r="I53" t="s">
+        <v>68</v>
+      </c>
+      <c r="J53" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54">
+        <f>0.98/1000</f>
+        <v>9.7999999999999997E-4</v>
+      </c>
+      <c r="C54" t="s">
+        <v>61</v>
+      </c>
+      <c r="D54" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" t="s">
+        <v>24</v>
+      </c>
+      <c r="I54" t="s">
+        <v>59</v>
+      </c>
+      <c r="J54" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>63</v>
+      </c>
+      <c r="B55">
+        <f>4.44/1000</f>
+        <v>4.4400000000000004E-3</v>
+      </c>
+      <c r="C55" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" t="s">
+        <v>24</v>
+      </c>
+      <c r="I55" t="s">
+        <v>59</v>
+      </c>
+      <c r="J55" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>42</v>
+      </c>
+      <c r="B56">
+        <v>0.42432000000000003</v>
+      </c>
+      <c r="C56" t="s">
+        <v>23</v>
+      </c>
+      <c r="D56" t="s">
+        <v>37</v>
+      </c>
+      <c r="F56" t="s">
+        <v>24</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>3.5360000000000001E-3</v>
+      </c>
+      <c r="I56" t="s">
+        <v>58</v>
+      </c>
+      <c r="J56" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>43</v>
+      </c>
+      <c r="B57">
+        <v>-0.50531999999999999</v>
+      </c>
+      <c r="C57" t="s">
+        <v>44</v>
+      </c>
+      <c r="D57" t="s">
+        <v>15</v>
+      </c>
+      <c r="F57" t="s">
+        <v>24</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>4.2110000000000003E-3</v>
+      </c>
+      <c r="I57" t="s">
+        <v>58</v>
+      </c>
+      <c r="J57" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>46</v>
+      </c>
+      <c r="B58">
+        <v>-0.22847999999999999</v>
+      </c>
+      <c r="C58" t="s">
+        <v>36</v>
+      </c>
+      <c r="D58" t="s">
+        <v>15</v>
+      </c>
+      <c r="F58" t="s">
+        <v>24</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>1.9040000000000001E-3</v>
+      </c>
+      <c r="I58" t="s">
+        <v>58</v>
+      </c>
+      <c r="J58" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>65</v>
+      </c>
+      <c r="B59" s="5">
+        <f>(-36.07/1000)+(-79/1000)</f>
+        <v>-0.11507000000000001</v>
+      </c>
+      <c r="C59" t="s">
+        <v>36</v>
+      </c>
+      <c r="D59" t="s">
+        <v>66</v>
+      </c>
+      <c r="F59" t="s">
+        <v>24</v>
+      </c>
+      <c r="I59" t="s">
+        <v>68</v>
+      </c>
+      <c r="J59" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>14</v>
+      </c>
+      <c r="B60">
+        <v>6.9264000000000001E-3</v>
+      </c>
+      <c r="D60" t="s">
+        <v>15</v>
+      </c>
+      <c r="E60" t="s">
+        <v>16</v>
+      </c>
+      <c r="F60" t="s">
+        <v>17</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>5.7720000000000003E-5</v>
+      </c>
+      <c r="I60" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>18</v>
       </c>
-      <c r="J26" t="s">
-        <v>53</v>
+      <c r="B61">
+        <v>2.48</v>
+      </c>
+      <c r="D61" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" t="s">
+        <v>16</v>
+      </c>
+      <c r="F61" t="s">
+        <v>17</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0.1502</v>
+      </c>
+      <c r="I61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62">
+        <v>1.0375199999999999E-2</v>
+      </c>
+      <c r="D62" t="s">
+        <v>15</v>
+      </c>
+      <c r="E62" t="s">
+        <v>16</v>
+      </c>
+      <c r="F62" t="s">
+        <v>17</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>8.6459999999999996E-5</v>
+      </c>
+      <c r="I62" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>82</v>
+      </c>
+      <c r="B63">
+        <f>17.77-B61</f>
+        <v>15.29</v>
+      </c>
+      <c r="C63" t="s">
+        <v>23</v>
+      </c>
+      <c r="D63" t="s">
+        <v>15</v>
+      </c>
+      <c r="F63" t="s">
+        <v>24</v>
+      </c>
+      <c r="I63" t="s">
+        <v>77</v>
+      </c>
+      <c r="J63" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J26" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:J25" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix hard coal input to coal-H2.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-coal-gasification.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-coal-gasification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6710E4D6-8A17-BE4B-9A51-9F74F63414F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6CE4A9-3F63-954E-8BFC-F29249B2DEF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -345,12 +345,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -635,7 +634,7 @@
   <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -715,7 +714,7 @@
       <c r="A10" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1121,7 +1120,7 @@
       <c r="A26" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="4">
         <f>-36.07/1000</f>
         <v>-3.6069999999999998E-2</v>
       </c>
@@ -1279,7 +1278,7 @@
       <c r="A38" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1559,7 +1558,7 @@
         <v>33</v>
       </c>
       <c r="B50">
-        <v>8.9</v>
+        <v>6.7709999999999999</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>52</v>
@@ -1809,7 +1808,7 @@
       <c r="A59" t="s">
         <v>65</v>
       </c>
-      <c r="B59" s="5">
+      <c r="B59" s="4">
         <f>(-36.07/1000)+(-79/1000)</f>
         <v>-0.11507000000000001</v>
       </c>

</xml_diff>

<commit_message>
Update inventories Improve correspondence of biosphere flows
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-coal-gasification.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-coal-gasification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33F0737-6B11-0D43-A8E2-8B6416514EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D50224-7A3C-5646-808C-FFD55C1A7CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37940" yWindow="1840" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37940" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$25</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="105">
   <si>
     <t>Activity</t>
   </si>
@@ -350,6 +350,9 @@
   </si>
   <si>
     <t>Carbon monoxide, fossil</t>
+  </si>
+  <si>
+    <t>hydrogen, gaseous, 30 bar</t>
   </si>
 </sst>
 </file>
@@ -359,9 +362,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -418,14 +428,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -749,8 +760,8 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>54</v>
+      <c r="B5" s="7" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -849,8 +860,8 @@
       <c r="I13" t="s">
         <v>21</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>54</v>
+      <c r="J13" s="7" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -1313,8 +1324,8 @@
       <c r="A33" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>54</v>
+      <c r="B33" s="7" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -1413,8 +1424,8 @@
       <c r="I41" t="s">
         <v>21</v>
       </c>
-      <c r="J41" s="2" t="s">
-        <v>54</v>
+      <c r="J41" s="7" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix issue relating to flow duplicates whn doing scenairo analysis
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-coal-gasification.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-coal-gasification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19933C8-544C-E948-92C4-A37A35CAC27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50002488-33AF-EF4A-BEE9-33009510AF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="1240" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="105">
   <si>
     <t>Activity</t>
   </si>
@@ -719,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1453,9 +1453,6 @@
         <f>32/1000</f>
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="C43" t="s">
-        <v>70</v>
-      </c>
       <c r="D43" t="s">
         <v>66</v>
       </c>

</xml_diff>